<commit_message>
Added create pivotChart using VBA
</commit_message>
<xml_diff>
--- a/Merged_Data.xlsx
+++ b/Merged_Data.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harvey\Desktop\Projects\csv_to_pivotChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E90761F-A19F-4A29-8A03-66AAC2D6228C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27D6575-CD0A-4903-B315-D97D9D7D2221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
-    <sheet name="Raw Data" sheetId="1" r:id="rId2"/>
+    <sheet name="PivotChart" sheetId="15" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Raw Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="197" r:id="rId3"/>
+    <pivotCache cacheId="120" r:id="rId4"/>
+    <pivotCache cacheId="125" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="15">
   <si>
     <t>Unit name</t>
   </si>
@@ -66,6 +68,9 @@
   </si>
   <si>
     <t>Unit_5</t>
+  </si>
+  <si>
+    <t>Average Current</t>
   </si>
 </sst>
 </file>
@@ -133,10 +138,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -202,6 +207,702 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Merged_Data.xlsx]PivotChart!MyPivotTable</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-PH"/>
+              <a:t>Average Current per Unit over Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PivotChart!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unit_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PivotChart!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10/1/2025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10/2/2025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10/3/2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10/4/2025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/5/2025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10/6/2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10/7/2025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10/8/2025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/9/2025</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10/10/2025</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PivotChart!$B$5:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.4990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.468</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8779999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.232</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.149</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4620000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84699999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E351-4663-8306-E6655E15B672}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PivotChart!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unit_2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PivotChart!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10/1/2025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10/2/2025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10/3/2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10/4/2025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/5/2025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10/6/2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10/7/2025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10/8/2025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/9/2025</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10/10/2025</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PivotChart!$C$5:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.4849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6319999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.40300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.046</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.577</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9059999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E351-4663-8306-E6655E15B672}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PivotChart!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unit_3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PivotChart!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10/1/2025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10/2/2025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10/3/2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10/4/2025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/5/2025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10/6/2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10/7/2025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10/8/2025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/9/2025</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10/10/2025</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PivotChart!$D$5:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.569</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7490000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0709999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.379</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.36599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1030000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1909999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E351-4663-8306-E6655E15B672}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PivotChart!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unit_4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PivotChart!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10/1/2025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10/2/2025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10/3/2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10/4/2025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/5/2025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10/6/2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10/7/2025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10/8/2025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/9/2025</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10/10/2025</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PivotChart!$E$5:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7610000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7720000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1629999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6509999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2120000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1789999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1280000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E351-4663-8306-E6655E15B672}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PivotChart!$F$3:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unit_5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PivotChart!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10/1/2025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10/2/2025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10/3/2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10/4/2025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/5/2025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10/6/2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10/7/2025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10/8/2025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/9/2025</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10/10/2025</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PivotChart!$F$5:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7610000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7720000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1629999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6509999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2120000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1789999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1280000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E351-4663-8306-E6655E15B672}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="30424304"/>
+        <c:axId val="30434864"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="30424304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="30434864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="30434864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="30424304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2369,16 +3070,57 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9E73BE5-67B6-C9CB-36F7-4792A7101BF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2407,7 +3149,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Harvey" refreshedDate="45942.562772337966" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="51" xr:uid="{98445A67-D682-40CF-8058-DFDE6A487146}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Harvey" refreshedDate="45942.850529745374" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="51" xr:uid="{98445A67-D682-40CF-8058-DFDE6A487146}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -2454,6 +3196,53 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Harvey" refreshedDate="45942.850654166665" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="51" xr:uid="{A6FD8774-9919-443F-A259-BF75654462E0}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:E52" sheet="Raw Data"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Unit name" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Unit_1"/>
+        <s v="Unit_2"/>
+        <s v="Unit_3"/>
+        <s v="Unit_4"/>
+        <s v="Unit_5"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="DateTime" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2025-10-01T00:00:00" maxDate="2025-10-11T00:00:00" count="10">
+        <d v="2025-10-01T00:00:00"/>
+        <d v="2025-10-02T00:00:00"/>
+        <d v="2025-10-03T00:00:00"/>
+        <d v="2025-10-04T00:00:00"/>
+        <d v="2025-10-05T00:00:00"/>
+        <d v="2025-10-06T00:00:00"/>
+        <d v="2025-10-07T00:00:00"/>
+        <d v="2025-10-08T00:00:00"/>
+        <d v="2025-10-09T00:00:00"/>
+        <d v="2025-10-10T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Voltage" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.0190000000000001" maxValue="4.1989999999999998"/>
+    </cacheField>
+    <cacheField name="Current" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.152" maxValue="4.9059999999999997"/>
+    </cacheField>
+    <cacheField name="Temperature" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="20.13" maxValue="44.95"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="51">
   <r>
@@ -2816,8 +3605,538 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="51">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.09"/>
+    <n v="1.4990000000000001"/>
+    <n v="30.68"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3.4620000000000002"/>
+    <n v="3.4180000000000001"/>
+    <n v="44.22"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3.2930000000000001"/>
+    <n v="3.468"/>
+    <n v="24.28"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="3.3740000000000001"/>
+    <n v="0.152"/>
+    <n v="44.95"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="3.726"/>
+    <n v="1.8779999999999999"/>
+    <n v="35.28"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="3.9860000000000002"/>
+    <n v="4.2290000000000001"/>
+    <n v="36.270000000000003"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="3.9689999999999999"/>
+    <n v="1.232"/>
+    <n v="38.17"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="7"/>
+    <n v="3.3279999999999998"/>
+    <n v="4.149"/>
+    <n v="33.57"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <n v="3.1230000000000002"/>
+    <n v="2.4620000000000002"/>
+    <n v="40.630000000000003"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <n v="3.2669999999999999"/>
+    <n v="0.84699999999999998"/>
+    <n v="24.47"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3.625"/>
+    <n v="3.4849999999999999"/>
+    <n v="31.79"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3.3650000000000002"/>
+    <n v="4.6319999999999997"/>
+    <n v="43.98"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3.1480000000000001"/>
+    <n v="4.3140000000000001"/>
+    <n v="30.4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3.3220000000000001"/>
+    <n v="0.40300000000000002"/>
+    <n v="43.7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="3.9670000000000001"/>
+    <n v="0.43"/>
+    <n v="29.96"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="3.3650000000000002"/>
+    <n v="0.36699999999999999"/>
+    <n v="41"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="3.774"/>
+    <n v="0.81100000000000005"/>
+    <n v="33.81"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="3.823"/>
+    <n v="1.046"/>
+    <n v="24.59"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="3.6949999999999998"/>
+    <n v="2.577"/>
+    <n v="27.07"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <n v="3.476"/>
+    <n v="4.9059999999999997"/>
+    <n v="21.9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3.597"/>
+    <n v="3.0449999999999999"/>
+    <n v="20.13"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3.5569999999999999"/>
+    <n v="2.569"/>
+    <n v="37.54"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3.2469999999999999"/>
+    <n v="3.5990000000000002"/>
+    <n v="37.93"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="3.6339999999999999"/>
+    <n v="3.7490000000000001"/>
+    <n v="34.26"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="3.355"/>
+    <n v="4.0709999999999997"/>
+    <n v="25.75"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="3.6760000000000002"/>
+    <n v="0.379"/>
+    <n v="37.020000000000003"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="3.101"/>
+    <n v="0.36599999999999999"/>
+    <n v="44.27"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="7"/>
+    <n v="3.7080000000000002"/>
+    <n v="0.42299999999999999"/>
+    <n v="44.68"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="8"/>
+    <n v="3.9769999999999999"/>
+    <n v="2.1030000000000002"/>
+    <n v="27.85"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="9"/>
+    <n v="3.4220000000000002"/>
+    <n v="3.1909999999999998"/>
+    <n v="37.51"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4.1769999999999996"/>
+    <n v="0.49299999999999999"/>
+    <n v="34.39"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4.1769999999999996"/>
+    <n v="0.49299999999999999"/>
+    <n v="34.39"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="3.0190000000000001"/>
+    <n v="4.7610000000000001"/>
+    <n v="29.26"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3.218"/>
+    <n v="4.7720000000000002"/>
+    <n v="21.44"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="4.0220000000000002"/>
+    <n v="3.1629999999999998"/>
+    <n v="39.659999999999997"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="3.6949999999999998"/>
+    <n v="3.6509999999999998"/>
+    <n v="29.93"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="4.1989999999999998"/>
+    <n v="2.08"/>
+    <n v="43.08"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="3.298"/>
+    <n v="3.25"/>
+    <n v="38.97"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="3.3940000000000001"/>
+    <n v="3.2120000000000002"/>
+    <n v="43.31"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="8"/>
+    <n v="3.0369999999999999"/>
+    <n v="3.1789999999999998"/>
+    <n v="28.03"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="9"/>
+    <n v="3.7149999999999999"/>
+    <n v="4.1280000000000001"/>
+    <n v="32.380000000000003"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="4.1769999999999996"/>
+    <n v="0.49299999999999999"/>
+    <n v="34.39"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3.0190000000000001"/>
+    <n v="4.7610000000000001"/>
+    <n v="29.26"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="3.218"/>
+    <n v="4.7720000000000002"/>
+    <n v="21.44"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="4.0220000000000002"/>
+    <n v="3.1629999999999998"/>
+    <n v="39.659999999999997"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="3.6949999999999998"/>
+    <n v="3.6509999999999998"/>
+    <n v="29.93"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <n v="4.1989999999999998"/>
+    <n v="2.08"/>
+    <n v="43.08"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="6"/>
+    <n v="3.298"/>
+    <n v="3.25"/>
+    <n v="38.97"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="7"/>
+    <n v="3.3940000000000001"/>
+    <n v="3.2120000000000002"/>
+    <n v="43.31"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="8"/>
+    <n v="3.0369999999999999"/>
+    <n v="3.1789999999999998"/>
+    <n v="28.03"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="9"/>
+    <n v="3.7149999999999999"/>
+    <n v="4.1280000000000001"/>
+    <n v="32.380000000000003"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62EBD2F5-653B-43E7-A7E6-5213E8FAE340}" name="PivotTable2" cacheId="197" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1EA63DB-01BF-4D3A-B63D-242E7F51371C}" name="MyPivotTable" cacheId="125" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:G15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average Current" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62EBD2F5-653B-43E7-A7E6-5213E8FAE340}" name="PivotTable2" cacheId="120" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A1:G13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -3325,6 +4644,315 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1367EBC0-76FE-4FE4-9B5F-5899F4797EB6}">
+  <sheetPr codeName="Sheet14"/>
+  <dimension ref="A3:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>45931</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1.4990000000000001</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3.4849999999999999</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3.0449999999999999</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1.5846666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>45932</v>
+      </c>
+      <c r="B6" s="7">
+        <v>3.4180000000000001</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4.6319999999999997</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2.569</v>
+      </c>
+      <c r="E6" s="7">
+        <v>4.7610000000000001</v>
+      </c>
+      <c r="F6" s="7">
+        <v>4.7610000000000001</v>
+      </c>
+      <c r="G6" s="7">
+        <v>4.0282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>45933</v>
+      </c>
+      <c r="B7" s="7">
+        <v>3.468</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4.3140000000000001</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4.7720000000000002</v>
+      </c>
+      <c r="F7" s="7">
+        <v>4.7720000000000002</v>
+      </c>
+      <c r="G7" s="7">
+        <v>4.1849999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>45934</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.152</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3.7490000000000001</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3.1629999999999998</v>
+      </c>
+      <c r="F8" s="7">
+        <v>3.1629999999999998</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2.1260000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>45935</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1.8779999999999999</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.43</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4.0709999999999997</v>
+      </c>
+      <c r="E9" s="7">
+        <v>3.6509999999999998</v>
+      </c>
+      <c r="F9" s="7">
+        <v>3.6509999999999998</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2.7361999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>45936</v>
+      </c>
+      <c r="B10" s="7">
+        <v>4.2290000000000001</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.379</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2.08</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2.08</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.827</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>45937</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1.232</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1.7818000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>45938</v>
+      </c>
+      <c r="B12" s="7">
+        <v>4.149</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1.046</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3.2120000000000002</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3.2120000000000002</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2.4083999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>45939</v>
+      </c>
+      <c r="B13" s="7">
+        <v>2.4620000000000002</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2.577</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2.1030000000000002</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3.1789999999999998</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3.1789999999999998</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>45940</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="C14" s="7">
+        <v>4.9059999999999997</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3.1909999999999998</v>
+      </c>
+      <c r="E14" s="7">
+        <v>4.1280000000000001</v>
+      </c>
+      <c r="F14" s="7">
+        <v>4.1280000000000001</v>
+      </c>
+      <c r="G14" s="7">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2.3334000000000001</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2.2970999999999995</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2.3494999999999999</v>
+      </c>
+      <c r="E15" s="7">
+        <v>3.016545454545454</v>
+      </c>
+      <c r="F15" s="7">
+        <v>3.2688999999999999</v>
+      </c>
+      <c r="G15" s="7">
+        <v>2.6602156862745101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278D68D0-742B-4E6D-A7BF-F39BE29529DC}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G13"/>
@@ -3379,22 +5007,22 @@
       <c r="A3" s="4">
         <v>45931</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>4.09</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>3.625</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <v>3.597</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <v>4.1769999999999996</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>4.1769999999999996</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="7">
         <v>3.9738333333333329</v>
       </c>
     </row>
@@ -3402,22 +5030,22 @@
       <c r="A4" s="4">
         <v>45932</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>3.4620000000000002</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>3.3650000000000002</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>3.5569999999999999</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <v>3.0190000000000001</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <v>3.0190000000000001</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <v>3.2844000000000002</v>
       </c>
     </row>
@@ -3425,22 +5053,22 @@
       <c r="A5" s="4">
         <v>45933</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>3.2930000000000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>3.1480000000000001</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>3.2469999999999999</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>3.218</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>3.218</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <v>3.2248000000000006</v>
       </c>
     </row>
@@ -3448,22 +5076,22 @@
       <c r="A6" s="4">
         <v>45934</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>3.3740000000000001</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>3.3220000000000001</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>3.6339999999999999</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>4.0220000000000002</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <v>4.0220000000000002</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <v>3.6748000000000003</v>
       </c>
     </row>
@@ -3471,22 +5099,22 @@
       <c r="A7" s="4">
         <v>45935</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>3.726</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>3.9670000000000001</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>3.355</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <v>3.6949999999999998</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="7">
         <v>3.6949999999999998</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="7">
         <v>3.6875999999999998</v>
       </c>
     </row>
@@ -3494,22 +5122,22 @@
       <c r="A8" s="4">
         <v>45936</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>3.9860000000000002</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>3.3650000000000002</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <v>3.6760000000000002</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>4.1989999999999998</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="7">
         <v>4.1989999999999998</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="7">
         <v>3.8850000000000002</v>
       </c>
     </row>
@@ -3517,22 +5145,22 @@
       <c r="A9" s="4">
         <v>45937</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>3.9689999999999999</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>3.774</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="7">
         <v>3.101</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <v>3.298</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="7">
         <v>3.298</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="7">
         <v>3.4880000000000004</v>
       </c>
     </row>
@@ -3540,22 +5168,22 @@
       <c r="A10" s="4">
         <v>45938</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <v>3.3279999999999998</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>3.823</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="7">
         <v>3.7080000000000002</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="7">
         <v>3.3940000000000001</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="7">
         <v>3.3940000000000001</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="7">
         <v>3.5293999999999999</v>
       </c>
     </row>
@@ -3563,22 +5191,22 @@
       <c r="A11" s="4">
         <v>45939</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <v>3.1230000000000002</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>3.6949999999999998</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="7">
         <v>3.9769999999999999</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="7">
         <v>3.0369999999999999</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="7">
         <v>3.0369999999999999</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="7">
         <v>3.3738000000000001</v>
       </c>
     </row>
@@ -3586,22 +5214,22 @@
       <c r="A12" s="4">
         <v>45940</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="7">
         <v>3.2669999999999999</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>3.476</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="7">
         <v>3.4220000000000002</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="7">
         <v>3.7149999999999999</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="7">
         <v>3.7149999999999999</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="7">
         <v>3.5189999999999997</v>
       </c>
     </row>
@@ -3609,22 +5237,22 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="7">
         <v>3.5618000000000003</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <v>3.556</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="7">
         <v>3.5274000000000001</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="7">
         <v>3.6319090909090903</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="7">
         <v>3.5773999999999999</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="7">
         <v>3.5720980392156862</v>
       </c>
     </row>
@@ -3634,13 +5262,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3656,7 +5284,7 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">

</xml_diff>